<commit_message>
Fix: Eliminación de errores en DataGrid y mejor ordenación
</commit_message>
<xml_diff>
--- a/public/data/nuevo_inventario.xlsx
+++ b/public/data/nuevo_inventario.xlsx
@@ -5,12 +5,12 @@
   <workbookPr hidePivotFieldList="1" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/martinbarroso/Library/CloudStorage/GoogleDrive-martin@simca.mx/Mi unidad/Martin Barroso/PUBLICO/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/martinbarroso/inventario-web/public/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EB427A05-530C-5345-A3F2-7107F39DE4AE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D29BF415-57A0-164E-BC4E-93111DDDE47D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="14400" windowHeight="17500" xr2:uid="{BAF3AA5D-A3F7-BA4A-95B0-71F6E6D7C4C4}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" xr2:uid="{BAF3AA5D-A3F7-BA4A-95B0-71F6E6D7C4C4}"/>
   </bookViews>
   <sheets>
     <sheet name="nombre_de_la_hoja" sheetId="1" r:id="rId1"/>
@@ -911,8 +911,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D42E4EA4-415E-AA45-8084-4CC1B58ADAC7}">
   <dimension ref="A1:I363"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A282" zoomScale="90" workbookViewId="0">
-      <selection activeCell="F306" sqref="F306"/>
+    <sheetView tabSelected="1" zoomScale="90" workbookViewId="0">
+      <selection activeCell="H32" sqref="H32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -926,23 +926,23 @@
     <col min="7" max="7" width="14" style="18" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="17.5" style="18" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="20" customWidth="1"/>
-    <col min="10" max="105" width="4.1640625" bestFit="1" customWidth="1"/>
-    <col min="106" max="106" width="5.83203125" bestFit="1" customWidth="1"/>
-    <col min="107" max="107" width="4.83203125" bestFit="1" customWidth="1"/>
-    <col min="108" max="116" width="5.83203125" bestFit="1" customWidth="1"/>
-    <col min="117" max="129" width="5.33203125" bestFit="1" customWidth="1"/>
-    <col min="130" max="131" width="5.83203125" bestFit="1" customWidth="1"/>
-    <col min="132" max="132" width="3.83203125" bestFit="1" customWidth="1"/>
-    <col min="133" max="134" width="5.83203125" bestFit="1" customWidth="1"/>
-    <col min="135" max="149" width="5.33203125" bestFit="1" customWidth="1"/>
-    <col min="150" max="150" width="5.6640625" bestFit="1" customWidth="1"/>
-    <col min="151" max="151" width="5.1640625" bestFit="1" customWidth="1"/>
-    <col min="152" max="152" width="4.1640625" bestFit="1" customWidth="1"/>
-    <col min="153" max="159" width="5.1640625" bestFit="1" customWidth="1"/>
-    <col min="160" max="164" width="6" bestFit="1" customWidth="1"/>
-    <col min="165" max="175" width="5.5" bestFit="1" customWidth="1"/>
-    <col min="176" max="176" width="3.1640625" bestFit="1" customWidth="1"/>
-    <col min="177" max="177" width="12" bestFit="1" customWidth="1"/>
+    <col min="10" max="104" width="4.1640625" bestFit="1" customWidth="1"/>
+    <col min="105" max="105" width="5.83203125" bestFit="1" customWidth="1"/>
+    <col min="106" max="106" width="4.83203125" bestFit="1" customWidth="1"/>
+    <col min="107" max="115" width="5.83203125" bestFit="1" customWidth="1"/>
+    <col min="116" max="128" width="5.33203125" bestFit="1" customWidth="1"/>
+    <col min="129" max="130" width="5.83203125" bestFit="1" customWidth="1"/>
+    <col min="131" max="131" width="3.83203125" bestFit="1" customWidth="1"/>
+    <col min="132" max="133" width="5.83203125" bestFit="1" customWidth="1"/>
+    <col min="134" max="148" width="5.33203125" bestFit="1" customWidth="1"/>
+    <col min="149" max="149" width="5.6640625" bestFit="1" customWidth="1"/>
+    <col min="150" max="150" width="5.1640625" bestFit="1" customWidth="1"/>
+    <col min="151" max="151" width="4.1640625" bestFit="1" customWidth="1"/>
+    <col min="152" max="158" width="5.1640625" bestFit="1" customWidth="1"/>
+    <col min="159" max="163" width="6" bestFit="1" customWidth="1"/>
+    <col min="164" max="174" width="5.5" bestFit="1" customWidth="1"/>
+    <col min="175" max="175" width="3.1640625" bestFit="1" customWidth="1"/>
+    <col min="176" max="176" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.2">
@@ -994,7 +994,6 @@
         <v>0.1</v>
       </c>
       <c r="G2" s="9">
-        <f>E2*F2</f>
         <v>46636.572444444442</v>
       </c>
       <c r="H2" s="31">
@@ -1022,7 +1021,6 @@
         <v>0.1</v>
       </c>
       <c r="G3" s="9">
-        <f>E3*F3</f>
         <v>43650.821058755093</v>
       </c>
       <c r="H3" s="31">
@@ -1050,7 +1048,6 @@
         <v>0.1</v>
       </c>
       <c r="G4" s="9">
-        <f>E4*F4</f>
         <v>43650.821058755093</v>
       </c>
       <c r="H4" s="31">
@@ -1078,7 +1075,6 @@
         <v>0.1</v>
       </c>
       <c r="G5" s="9">
-        <f>E5*F5</f>
         <v>55529.369774166684</v>
       </c>
       <c r="H5" s="31">
@@ -1106,7 +1102,6 @@
         <v>0.1</v>
       </c>
       <c r="G6" s="9">
-        <f>E6*F6</f>
         <v>43650.821058755093</v>
       </c>
       <c r="H6" s="31">
@@ -1134,7 +1129,6 @@
         <v>0.1</v>
       </c>
       <c r="G7" s="9">
-        <f>E7*F7</f>
         <v>55529.369774166684</v>
       </c>
       <c r="H7" s="31">
@@ -1162,7 +1156,6 @@
         <v>0.1</v>
       </c>
       <c r="G8" s="9">
-        <f>E8*F8</f>
         <v>46675.277312390928</v>
       </c>
       <c r="H8" s="31">
@@ -1190,7 +1183,6 @@
         <v>0.1</v>
       </c>
       <c r="G9" s="9">
-        <f>E9*F9</f>
         <v>56930.052777222234</v>
       </c>
       <c r="H9" s="31">
@@ -1218,7 +1210,6 @@
         <v>0.1</v>
       </c>
       <c r="G10" s="9">
-        <f>E10*F10</f>
         <v>46675.277312390928</v>
       </c>
       <c r="H10" s="31">
@@ -1246,7 +1237,6 @@
         <v>0.1</v>
       </c>
       <c r="G11" s="9">
-        <f>E11*F11</f>
         <v>56930.052777222234</v>
       </c>
       <c r="H11" s="31">
@@ -1274,7 +1264,6 @@
         <v>0.1</v>
       </c>
       <c r="G12" s="9">
-        <f>E12*F12</f>
         <v>46675.277312390928</v>
       </c>
       <c r="H12" s="31">
@@ -1302,7 +1291,6 @@
         <v>0.1</v>
       </c>
       <c r="G13" s="9">
-        <f>E13*F13</f>
         <v>58330.736830555572</v>
       </c>
       <c r="H13" s="31">
@@ -1330,7 +1318,6 @@
         <v>0.1</v>
       </c>
       <c r="G14" s="9">
-        <f>E14*F14</f>
         <v>58330.736830555572</v>
       </c>
       <c r="H14" s="31">
@@ -1358,7 +1345,6 @@
         <v>0.1</v>
       </c>
       <c r="G15" s="9">
-        <f>E15*F15</f>
         <v>59830.400000000001</v>
       </c>
       <c r="H15" s="31">
@@ -1386,7 +1372,6 @@
         <v>0.1</v>
       </c>
       <c r="G16" s="9">
-        <f>E16*F16</f>
         <v>47463.3</v>
       </c>
       <c r="H16" s="31">
@@ -1414,7 +1399,6 @@
         <v>0.1</v>
       </c>
       <c r="G17" s="9">
-        <f>E17*F17</f>
         <v>70103.591368611131</v>
       </c>
       <c r="H17" s="31">
@@ -1442,7 +1426,6 @@
         <v>0.1</v>
       </c>
       <c r="G18" s="9">
-        <f>E18*F18</f>
         <v>81113.374989444448</v>
       </c>
       <c r="H18" s="31">
@@ -1470,7 +1453,6 @@
         <v>0.1</v>
       </c>
       <c r="G19" s="9">
-        <f>E19*F19</f>
         <v>70103.591368611131</v>
       </c>
       <c r="H19" s="31">
@@ -1498,7 +1480,6 @@
         <v>0.1</v>
       </c>
       <c r="G20" s="9">
-        <f>E20*F20</f>
         <v>81113.374989444448</v>
       </c>
       <c r="H20" s="31">
@@ -1526,7 +1507,6 @@
         <v>0.2</v>
       </c>
       <c r="G21" s="11">
-        <f>E21*F21</f>
         <v>157980</v>
       </c>
       <c r="H21" s="31">
@@ -1554,7 +1534,6 @@
         <v>0.2</v>
       </c>
       <c r="G22" s="16">
-        <f>E22*F22</f>
         <v>100980</v>
       </c>
       <c r="H22" s="31">
@@ -1582,7 +1561,6 @@
         <v>0.2</v>
       </c>
       <c r="G23" s="16">
-        <f>E23*F23</f>
         <v>99980</v>
       </c>
       <c r="H23" s="31">
@@ -1610,7 +1588,6 @@
         <v>0.2</v>
       </c>
       <c r="G24" s="16">
-        <f>E24*F24</f>
         <v>94980</v>
       </c>
       <c r="H24" s="31">
@@ -1638,7 +1615,6 @@
         <v>0.2</v>
       </c>
       <c r="G25" s="16">
-        <f>E25*F25</f>
         <v>103980</v>
       </c>
       <c r="H25" s="31">
@@ -1666,7 +1642,6 @@
         <v>0.2</v>
       </c>
       <c r="G26" s="16">
-        <f>E26*F26</f>
         <v>94880</v>
       </c>
       <c r="H26" s="31">
@@ -1694,7 +1669,6 @@
         <v>0.2</v>
       </c>
       <c r="G27" s="16">
-        <f>E27*F27</f>
         <v>109340</v>
       </c>
       <c r="H27" s="31">
@@ -1722,7 +1696,6 @@
         <v>0.2</v>
       </c>
       <c r="G28" s="16">
-        <f>E28*F28</f>
         <v>94880</v>
       </c>
       <c r="H28" s="31">
@@ -1750,7 +1723,6 @@
         <v>0.2</v>
       </c>
       <c r="G29" s="16">
-        <f>E29*F29</f>
         <v>172980</v>
       </c>
       <c r="H29" s="31">
@@ -1778,7 +1750,6 @@
         <v>0.2</v>
       </c>
       <c r="G30" s="16">
-        <f>E30*F30</f>
         <v>105860</v>
       </c>
       <c r="H30" s="31">
@@ -1806,7 +1777,6 @@
         <v>0.2</v>
       </c>
       <c r="G31" s="16">
-        <f>E31*F31</f>
         <v>93980</v>
       </c>
       <c r="H31" s="31">
@@ -1834,7 +1804,6 @@
         <v>0.2</v>
       </c>
       <c r="G32" s="16">
-        <f>E32*F32</f>
         <v>105980</v>
       </c>
       <c r="H32" s="31">
@@ -1862,7 +1831,6 @@
         <v>0.2</v>
       </c>
       <c r="G33" s="16">
-        <f>E33*F33</f>
         <v>93860</v>
       </c>
       <c r="H33" s="31">
@@ -1890,7 +1858,6 @@
         <v>0.2</v>
       </c>
       <c r="G34" s="16">
-        <f>E34*F34</f>
         <v>90800</v>
       </c>
       <c r="H34" s="31">
@@ -1918,7 +1885,6 @@
         <v>0.2</v>
       </c>
       <c r="G35" s="16">
-        <f>E35*F35</f>
         <v>109980</v>
       </c>
       <c r="H35" s="31">
@@ -1946,7 +1912,6 @@
         <v>0.2</v>
       </c>
       <c r="G36" s="16">
-        <f>E36*F36</f>
         <v>155100</v>
       </c>
       <c r="H36" s="31">
@@ -1974,7 +1939,6 @@
         <v>0.2</v>
       </c>
       <c r="G37" s="16">
-        <f>E37*F37</f>
         <v>93980</v>
       </c>
       <c r="H37" s="31">
@@ -2002,7 +1966,6 @@
         <v>0.2</v>
       </c>
       <c r="G38" s="16">
-        <f>E38*F38</f>
         <v>88980</v>
       </c>
       <c r="H38" s="31">
@@ -2057,7 +2020,6 @@
         <v>0.2</v>
       </c>
       <c r="G40" s="16">
-        <f>E40*F40</f>
         <v>95980</v>
       </c>
       <c r="H40" s="31">
@@ -2085,7 +2047,6 @@
         <v>0.2</v>
       </c>
       <c r="G41" s="16">
-        <f>E41*F41</f>
         <v>97980</v>
       </c>
       <c r="H41" s="31">
@@ -3654,7 +3615,6 @@
         <v>0.15</v>
       </c>
       <c r="G109" s="11">
-        <f>E109*F109</f>
         <v>133862.60294117648</v>
       </c>
       <c r="H109" s="31">
@@ -3682,7 +3642,6 @@
         <v>0.15</v>
       </c>
       <c r="G110" s="11">
-        <f>E110*F110</f>
         <v>133862.60294117648</v>
       </c>
       <c r="H110" s="31">
@@ -3710,7 +3669,6 @@
         <v>0.15</v>
       </c>
       <c r="G111" s="11">
-        <f>E111*F111</f>
         <v>233709.26647058825</v>
       </c>
       <c r="H111" s="31">
@@ -3738,7 +3696,6 @@
         <v>0.15</v>
       </c>
       <c r="G112" s="11">
-        <f>E112*F112</f>
         <v>189232.11529411766</v>
       </c>
       <c r="H112" s="31">
@@ -3766,7 +3723,6 @@
         <v>0.15</v>
       </c>
       <c r="G113" s="11">
-        <f>E113*F113</f>
         <v>194224.45058823531</v>
       </c>
       <c r="H113" s="31">
@@ -3794,7 +3750,6 @@
         <v>0.15</v>
       </c>
       <c r="G114" s="11">
-        <f>E114*F114</f>
         <v>196947.54</v>
       </c>
       <c r="H114" s="31">
@@ -3822,7 +3777,6 @@
         <v>0.15</v>
       </c>
       <c r="G115" s="11">
-        <f>E115*F115</f>
         <v>119339.45294117647</v>
       </c>
       <c r="H115" s="31">
@@ -4487,7 +4441,6 @@
         <v>0.2</v>
       </c>
       <c r="G143" s="12">
-        <f>E143*F143</f>
         <v>123900</v>
       </c>
       <c r="H143" s="31">
@@ -4596,7 +4549,6 @@
         <v>0.2</v>
       </c>
       <c r="G147" s="12">
-        <f>E147*F147</f>
         <v>124940</v>
       </c>
       <c r="H147" s="31">
@@ -4678,7 +4630,6 @@
         <v>0.2</v>
       </c>
       <c r="G150" s="11">
-        <f>E150*F150</f>
         <v>118000</v>
       </c>
       <c r="H150" s="31">
@@ -9418,7 +9369,6 @@
         <v>0.06</v>
       </c>
       <c r="G350" s="11">
-        <f>E350*F350</f>
         <v>28505.52</v>
       </c>
       <c r="H350" s="31">

</xml_diff>